<commit_message>
Discussion on Nomenclature for EconomicDispatch
</commit_message>
<xml_diff>
--- a/Book chapter Studies/Data to optimization/Parameters table.xlsx
+++ b/Book chapter Studies/Data to optimization/Parameters table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szata\Codes\StoriesTeams\Pipeline-dispatcher\Book chapter Studies\Data to optimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kheu\git\stories\Pipeline-dispatcher\Book chapter Studies\Data to optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3084C4-0C62-485F-9B01-9AEC32D26B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8195F799-4CA4-417C-BFA5-7948B926DAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{A72227BA-6150-4B49-869F-1EC4BCBCAEF0}"/>
+    <workbookView xWindow="-57720" yWindow="-6615" windowWidth="29040" windowHeight="17790" xr2:uid="{A72227BA-6150-4B49-869F-1EC4BCBCAEF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Data structure" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="261">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -709,6 +709,118 @@
   </si>
   <si>
     <t>Name+B48:B55</t>
+  </si>
+  <si>
+    <t>Variable Name in Economic Dispatch</t>
+  </si>
+  <si>
+    <t>pBat_1</t>
+  </si>
+  <si>
+    <t>transdict['BAT_ESSm_PP']</t>
+  </si>
+  <si>
+    <t>for var_name in trans_dict.keys:
+   ecodispdata_dict[transdict[var_name]] = scenariodata[var_name]</t>
+  </si>
+  <si>
+    <t>pBti,t Net basepoint power of ESS i at time t</t>
+  </si>
+  <si>
+    <t>pBtchi,t Charging power of ESS i at time t</t>
+  </si>
+  <si>
+    <t>pBtdisi,t Discharging power of ESS i at time t</t>
+  </si>
+  <si>
+    <t>zchi,t Binary variable: 1 if ESS i is charging at t</t>
+  </si>
+  <si>
+    <t>zdisi,t Binary variable: 1 if ESS i is discharging at t</t>
+  </si>
+  <si>
+    <t>eti,t State of charge of ESS i at time t</t>
+  </si>
+  <si>
+    <t>et0i Initial state of charge of ESS i</t>
+  </si>
+  <si>
+    <t>EImp</t>
+  </si>
+  <si>
+    <t>t Energy imported from the grid at time t</t>
+  </si>
+  <si>
+    <t>EExp</t>
+  </si>
+  <si>
+    <t>t Energy exported to the grid at time t</t>
+  </si>
+  <si>
+    <t>P Imp</t>
+  </si>
+  <si>
+    <t>t Power imported from the grid at time t</t>
+  </si>
+  <si>
+    <t>P Exp</t>
+  </si>
+  <si>
+    <t>t Power exported to the grid at time t</t>
+  </si>
+  <si>
+    <t>pRC</t>
+  </si>
+  <si>
+    <t>t Power generated from Rankine cycle at time t</t>
+  </si>
+  <si>
+    <t>P Gen</t>
+  </si>
+  <si>
+    <t>t Total power generation at time t</t>
+  </si>
+  <si>
+    <t>P Load</t>
+  </si>
+  <si>
+    <t>t Total electrical load at time t</t>
+  </si>
+  <si>
+    <t>P Cbu</t>
+  </si>
+  <si>
+    <t>t Electrical load of controllable building units at time t</t>
+  </si>
+  <si>
+    <t>P Cebu</t>
+  </si>
+  <si>
+    <t>t Electrical load of controllable equipment building units at time t</t>
+  </si>
+  <si>
+    <t>P EV</t>
+  </si>
+  <si>
+    <t>t EV charging/discharging power at time t</t>
+  </si>
+  <si>
+    <t>P P elletizer</t>
+  </si>
+  <si>
+    <t>t Power consumption of pelletizer at time t</t>
+  </si>
+  <si>
+    <t>P P V</t>
+  </si>
+  <si>
+    <t>t Power from photovoltaics at time t</t>
+  </si>
+  <si>
+    <t>P W ind</t>
+  </si>
+  <si>
+    <t>t Power from wind at time t</t>
   </si>
 </sst>
 </file>
@@ -984,7 +1096,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1055,6 +1167,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1470,23 +1586,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB92B14-1692-4C09-8448-4C4DAA882D37}">
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="42" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="55.42578125" customWidth="1"/>
     <col min="7" max="7" width="54.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>218</v>
       </c>
@@ -1495,16 +1611,16 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
       <c r="E2" s="55" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>219</v>
       </c>
@@ -1518,11 +1634,14 @@
       <c r="H3" s="14"/>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="58"/>
+      <c r="B4" s="57" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="58"/>
       <c r="E4" s="16"/>
       <c r="F4" s="17" t="s">
         <v>206</v>
@@ -1531,11 +1650,12 @@
       <c r="H4" s="18"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="56"/>
+      <c r="C5" s="50" t="s">
         <v>108</v>
       </c>
       <c r="E5" s="20"/>
@@ -1548,11 +1668,11 @@
       <c r="H5" s="22"/>
       <c r="I5" s="23"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="C6" s="25" t="s">
         <v>125</v>
       </c>
       <c r="E6" s="24"/>
@@ -1564,11 +1684,11 @@
       </c>
       <c r="I6" s="25"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="C7" s="25" t="s">
         <v>125</v>
       </c>
       <c r="E7" s="24"/>
@@ -1580,11 +1700,11 @@
       </c>
       <c r="I7" s="25"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="C8" s="25" t="s">
         <v>125</v>
       </c>
       <c r="E8" s="24"/>
@@ -1596,11 +1716,11 @@
       </c>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="C9" s="25" t="s">
         <v>125</v>
       </c>
       <c r="E9" s="24"/>
@@ -1611,13 +1731,19 @@
         <v>191</v>
       </c>
       <c r="I9" s="25"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="C10" s="25" t="s">
         <v>125</v>
+      </c>
+      <c r="D10" t="s">
+        <v>226</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10" t="s">
@@ -1627,13 +1753,22 @@
         <v>193</v>
       </c>
       <c r="I10" s="25"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>125</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>227</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" t="s">
@@ -1643,12 +1778,15 @@
         <v>195</v>
       </c>
       <c r="I11" s="25"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="C12" s="25" t="s">
         <v>125</v>
       </c>
       <c r="E12" s="24"/>
@@ -1659,12 +1797,15 @@
         <v>197</v>
       </c>
       <c r="I12" s="25"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="C13" s="25" t="s">
         <v>125</v>
       </c>
       <c r="E13" s="24"/>
@@ -1675,12 +1816,15 @@
         <v>104</v>
       </c>
       <c r="I13" s="25"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="C14" s="25" t="s">
         <v>125</v>
       </c>
       <c r="E14" s="24"/>
@@ -1691,12 +1835,15 @@
         <v>210</v>
       </c>
       <c r="I14" s="25"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="C15" s="25" t="s">
         <v>125</v>
       </c>
       <c r="E15" s="24"/>
@@ -1707,12 +1854,15 @@
         <v>211</v>
       </c>
       <c r="I15" s="25"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="C16" s="25" t="s">
         <v>125</v>
       </c>
       <c r="E16" s="24"/>
@@ -1723,12 +1873,15 @@
         <v>214</v>
       </c>
       <c r="I16" s="25"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="C17" s="25" t="s">
         <v>125</v>
       </c>
       <c r="E17" s="24"/>
@@ -1739,12 +1892,15 @@
         <v>208</v>
       </c>
       <c r="I17" s="25"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="C18" s="25" t="s">
         <v>125</v>
       </c>
       <c r="E18" s="24"/>
@@ -1755,12 +1911,15 @@
         <v>213</v>
       </c>
       <c r="I18" s="25"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="C19" s="25" t="s">
         <v>128</v>
       </c>
       <c r="E19" s="24"/>
@@ -1771,12 +1930,15 @@
         <v>215</v>
       </c>
       <c r="I19" s="25"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="C20" s="54" t="s">
         <v>131</v>
       </c>
       <c r="E20" s="24"/>
@@ -1787,8 +1949,11 @@
         <v>212</v>
       </c>
       <c r="I20" s="25"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="59" t="s">
         <v>220</v>
       </c>
@@ -1800,12 +1965,18 @@
         <v>209</v>
       </c>
       <c r="I21" s="25"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="B22" s="58"/>
+      <c r="B22" s="57" t="s">
+        <v>224</v>
+      </c>
+      <c r="C22" s="58"/>
       <c r="E22" s="16"/>
       <c r="F22" s="17" t="s">
         <v>129</v>
@@ -1813,12 +1984,15 @@
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
       <c r="I22" s="19"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="C23" s="50" t="s">
         <v>108</v>
       </c>
       <c r="E23" s="20"/>
@@ -1830,12 +2004,15 @@
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="23"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="C24" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E24" s="24"/>
@@ -1846,12 +2023,15 @@
         <v>78</v>
       </c>
       <c r="I24" s="25"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="C25" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E25" s="24"/>
@@ -1862,12 +2042,15 @@
         <v>80</v>
       </c>
       <c r="I25" s="25"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="C26" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E26" s="24"/>
@@ -1878,12 +2061,15 @@
         <v>82</v>
       </c>
       <c r="I26" s="25"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="C27" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E27" s="24"/>
@@ -1894,12 +2080,15 @@
         <v>84</v>
       </c>
       <c r="I27" s="25"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="C28" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E28" s="24"/>
@@ -1910,12 +2099,15 @@
         <v>86</v>
       </c>
       <c r="I28" s="25"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="C29" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E29" s="24"/>
@@ -1926,12 +2118,15 @@
         <v>86</v>
       </c>
       <c r="I29" s="25"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="C30" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E30" s="24"/>
@@ -1942,12 +2137,15 @@
         <v>88</v>
       </c>
       <c r="I30" s="25"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="C31" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E31" s="24"/>
@@ -1958,12 +2156,15 @@
         <v>90</v>
       </c>
       <c r="I31" s="25"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="C32" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E32" s="24"/>
@@ -1974,12 +2175,15 @@
         <v>92</v>
       </c>
       <c r="I32" s="25"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="C33" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E33" s="24"/>
@@ -1990,12 +2194,15 @@
         <v>94</v>
       </c>
       <c r="I33" s="25"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="C34" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E34" s="24"/>
@@ -2006,12 +2213,15 @@
         <v>96</v>
       </c>
       <c r="I34" s="25"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="C35" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E35" s="24"/>
@@ -2022,12 +2232,15 @@
         <v>98</v>
       </c>
       <c r="I35" s="25"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="C36" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E36" s="24"/>
@@ -2038,12 +2251,15 @@
         <v>100</v>
       </c>
       <c r="I36" s="25"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="C37" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E37" s="24"/>
@@ -2054,12 +2270,16 @@
         <v>102</v>
       </c>
       <c r="I37" s="25"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="60"/>
+      <c r="C38" s="25" t="s">
         <v>175</v>
       </c>
       <c r="E38" s="24"/>
@@ -2070,12 +2290,16 @@
         <v>104</v>
       </c>
       <c r="I38" s="25"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K38" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="60"/>
+      <c r="C39" s="25" t="s">
         <v>175</v>
       </c>
       <c r="E39" s="24"/>
@@ -2086,12 +2310,16 @@
         <v>106</v>
       </c>
       <c r="I39" s="25"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="60"/>
+      <c r="C40" s="25" t="s">
         <v>175</v>
       </c>
       <c r="E40" s="16"/>
@@ -2101,12 +2329,16 @@
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
       <c r="I40" s="19"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="60"/>
+      <c r="C41" s="25" t="s">
         <v>175</v>
       </c>
       <c r="E41" s="32" t="s">
@@ -2122,12 +2354,15 @@
       <c r="I41" s="23" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="C42" s="25" t="s">
         <v>175</v>
       </c>
       <c r="E42" s="35" t="s">
@@ -2146,11 +2381,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="B43" s="25" t="s">
+      <c r="C43" s="25" t="s">
         <v>175</v>
       </c>
       <c r="E43" s="35"/>
@@ -2167,11 +2402,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="B44" s="25" t="s">
+      <c r="C44" s="25" t="s">
         <v>175</v>
       </c>
       <c r="E44" s="35"/>
@@ -2188,11 +2423,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="C45" s="25" t="s">
         <v>175</v>
       </c>
       <c r="E45" s="35"/>
@@ -2207,11 +2442,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="B46" s="25" t="s">
+      <c r="C46" s="25" t="s">
         <v>175</v>
       </c>
       <c r="E46" s="35"/>
@@ -2226,11 +2461,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="B47" s="25" t="s">
+      <c r="C47" s="25" t="s">
         <v>175</v>
       </c>
       <c r="E47" s="35" t="s">
@@ -2249,11 +2484,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="B48" s="25" t="s">
+      <c r="C48" s="25" t="s">
         <v>126</v>
       </c>
       <c r="E48" s="35"/>
@@ -2274,7 +2509,7 @@
       <c r="A49" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="C49" s="25" t="s">
         <v>126</v>
       </c>
       <c r="E49" s="35"/>
@@ -2295,7 +2530,7 @@
       <c r="A50" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="B50" s="25" t="s">
+      <c r="C50" s="25" t="s">
         <v>126</v>
       </c>
       <c r="E50" s="35"/>
@@ -2316,7 +2551,7 @@
       <c r="A51" s="52" t="s">
         <v>159</v>
       </c>
-      <c r="B51" s="25" t="s">
+      <c r="C51" s="25" t="s">
         <v>126</v>
       </c>
       <c r="E51" s="35"/>
@@ -2337,7 +2572,7 @@
       <c r="A52" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="B52" s="25" t="s">
+      <c r="C52" s="25" t="s">
         <v>126</v>
       </c>
       <c r="E52" s="32" t="s">
@@ -2354,7 +2589,7 @@
       <c r="A53" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="B53" s="25" t="s">
+      <c r="C53" s="25" t="s">
         <v>126</v>
       </c>
       <c r="E53" s="24">
@@ -2374,7 +2609,7 @@
       <c r="A54" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="B54" s="25" t="s">
+      <c r="C54" s="25" t="s">
         <v>126</v>
       </c>
       <c r="E54" s="41">
@@ -2397,7 +2632,7 @@
       <c r="A55" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="B55" s="25" t="s">
+      <c r="C55" s="25" t="s">
         <v>223</v>
       </c>
       <c r="E55" s="41">
@@ -2420,7 +2655,7 @@
       <c r="A56" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="B56" s="25" t="s">
+      <c r="C56" s="25" t="s">
         <v>126</v>
       </c>
       <c r="E56" s="41">
@@ -2443,7 +2678,7 @@
       <c r="A57" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="B57" s="25" t="s">
+      <c r="C57" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E57" s="41">
@@ -2466,7 +2701,7 @@
       <c r="A58" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="C58" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E58" s="41">
@@ -2489,7 +2724,7 @@
       <c r="A59" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="B59" s="25" t="s">
+      <c r="C59" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E59" s="41">
@@ -2512,7 +2747,7 @@
       <c r="A60" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="B60" s="25" t="s">
+      <c r="C60" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E60" s="41">
@@ -2535,7 +2770,7 @@
       <c r="A61" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B61" s="25" t="s">
+      <c r="C61" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E61" s="41">
@@ -2558,7 +2793,7 @@
       <c r="A62" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="B62" s="25" t="s">
+      <c r="C62" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E62" s="41">
@@ -2581,7 +2816,7 @@
       <c r="A63" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="B63" s="25" t="s">
+      <c r="C63" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E63" s="41">
@@ -2604,7 +2839,7 @@
       <c r="A64" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="B64" s="25" t="s">
+      <c r="C64" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E64" s="41">
@@ -2627,7 +2862,7 @@
       <c r="A65" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="C65" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E65" s="41">
@@ -2650,7 +2885,7 @@
       <c r="A66" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B66" s="25" t="s">
+      <c r="C66" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E66" s="41">
@@ -2673,7 +2908,7 @@
       <c r="A67" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B67" s="54" t="s">
+      <c r="C67" s="54" t="s">
         <v>38</v>
       </c>
       <c r="E67" s="41">
@@ -2716,7 +2951,7 @@
       <c r="A69" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="B69" s="58"/>
+      <c r="C69" s="58"/>
       <c r="E69" s="41">
         <v>16</v>
       </c>
@@ -2735,7 +2970,7 @@
       <c r="A70" s="51" t="s">
         <v>181</v>
       </c>
-      <c r="B70" s="50" t="s">
+      <c r="C70" s="50" t="s">
         <v>108</v>
       </c>
       <c r="E70" s="42">
@@ -2756,7 +2991,7 @@
       <c r="A71" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B71" s="25" t="s">
+      <c r="C71" s="25" t="s">
         <v>216</v>
       </c>
       <c r="E71" s="43">
@@ -2779,7 +3014,7 @@
       <c r="A72" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B72" s="25" t="s">
+      <c r="C72" s="25" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2787,7 +3022,7 @@
       <c r="A73" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B73" s="25" t="s">
+      <c r="C73" s="25" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2795,7 +3030,7 @@
       <c r="A74" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B74" s="25" t="s">
+      <c r="C74" s="25" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2803,7 +3038,7 @@
       <c r="A75" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B75" s="25" t="s">
+      <c r="C75" s="25" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2811,7 +3046,7 @@
       <c r="A76" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B76" s="25" t="s">
+      <c r="C76" s="25" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2819,7 +3054,7 @@
       <c r="A77" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B77" s="25" t="s">
+      <c r="C77" s="25" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2827,7 +3062,7 @@
       <c r="A78" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B78" s="25" t="s">
+      <c r="C78" s="25" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2835,7 +3070,7 @@
       <c r="A79" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B79" s="25" t="s">
+      <c r="C79" s="25" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2843,93 +3078,93 @@
       <c r="A80" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B80" s="25" t="s">
+      <c r="C80" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B81" s="25" t="s">
+      <c r="C81" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B82" s="25" t="s">
+      <c r="C82" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B83" s="25" t="s">
+      <c r="C83" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B84" s="25" t="s">
+      <c r="C84" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B85" s="25" t="s">
+      <c r="C85" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B86" s="25" t="s">
+      <c r="C86" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B87" s="25" t="s">
+      <c r="C87" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B88" s="25" t="s">
+      <c r="C88" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="B89" s="25" t="s">
+      <c r="C89" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="53" t="s">
         <v>216</v>
       </c>
-      <c r="B90" s="54" t="s">
+      <c r="C90" s="54" t="s">
         <v>216</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="A24:A65 A68">
+  <conditionalFormatting sqref="A68:B68 A24:B65">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
@@ -2970,6 +3205,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>